<commit_message>
add group config management
</commit_message>
<xml_diff>
--- a/temp_downloads/全院收入_按科室202501门诊-开单科室 copy_processed.xlsx
+++ b/temp_downloads/全院收入_按科室202501门诊-开单科室 copy_processed.xlsx
@@ -426,7 +426,7 @@
   <cols>
     <col width="40" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
@@ -707,7 +707,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>医疗服务性收入合计</t>
+          <t>医疗服务性收入合计，测试表头</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">

</xml_diff>